<commit_message>
merged and fixed conflicts
</commit_message>
<xml_diff>
--- a/Expert_Elicitation/expertelicitation_table.xlsx
+++ b/Expert_Elicitation/expertelicitation_table.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4060" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="24600" yWindow="-19340" windowWidth="25600" windowHeight="15480" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="expertelictation" sheetId="1" r:id="rId1"/>
     <sheet name="plots" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="59">
   <si>
     <t>Variable</t>
   </si>
@@ -201,6 +202,12 @@
   </si>
   <si>
     <t>var_logitscale</t>
+  </si>
+  <si>
+    <t>Regional Differences</t>
+  </si>
+  <si>
+    <t>region1</t>
   </si>
 </sst>
 </file>
@@ -861,11 +868,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2121095544"/>
-        <c:axId val="2121097592"/>
+        <c:axId val="2092083592"/>
+        <c:axId val="2093447896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2121095544"/>
+        <c:axId val="2092083592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -893,12 +900,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121097592"/>
+        <c:crossAx val="2093447896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2121097592"/>
+        <c:axId val="2093447896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -926,7 +933,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121095544"/>
+        <c:crossAx val="2092083592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1304,7 +1311,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -2590,4 +2597,37 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>